<commit_message>
Modified validation of testcases in AppBridgeTestData.xlsx
</commit_message>
<xml_diff>
--- a/src/test/test-data/AppBridgeTestData.xlsx
+++ b/src/test/test-data/AppBridgeTestData.xlsx
@@ -99,9 +99,6 @@
     <t>status=200||truid=(SYS_USER1)||errorCode=ab-error-102||errorMsg=error out when retrieving endnote token</t>
   </si>
   <si>
-    <t>status=200||truid=(SYS_USER1)||enRedirectUrl=http://app.qc.endnote.com/auth?token</t>
-  </si>
-  <si>
     <t>OPQA-896</t>
   </si>
   <si>
@@ -238,6 +235,9 @@
   </si>
   <si>
     <t>OPQA-XXXX10</t>
+  </si>
+  <si>
+    <t>status=200||truid=(SYS_USER1)||enRedirectUrl=https://app.qc.endnote.com/auth?token</t>
   </si>
 </sst>
 </file>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E9" workbookViewId="0">
-      <selection activeCell="L14" sqref="L2:L14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -719,7 +719,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" s="5" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="K2" s="1"/>
     </row>
@@ -771,194 +771,194 @@
     </row>
     <row r="5" spans="1:12" ht="45">
       <c r="A5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>31</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
       <c r="J5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H6"/>
       <c r="I6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75">
       <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
       <c r="J7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="45">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H8"/>
       <c r="I8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="1"/>
       <c r="J9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45">
       <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H10"/>
       <c r="I10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="60">
       <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H11"/>
       <c r="I11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>19</v>
@@ -966,24 +966,24 @@
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>37</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>38</v>
       </c>
       <c r="F12" s="1"/>
       <c r="H12"/>
       <c r="I12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>23</v>
@@ -991,56 +991,56 @@
     </row>
     <row r="13" spans="1:12" ht="45">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H13"/>
       <c r="I13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="45">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H14"/>
       <c r="I14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1136,58 +1136,58 @@
     </row>
     <row r="3" spans="1:12" ht="15.75">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="60">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1262,7 +1262,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>
@@ -1277,63 +1277,63 @@
         <v>15</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="60">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created Class for Steam down, created testcases in Jira for AppBridge and Oauth excels updated in excel with testcase Ids
</commit_message>
<xml_diff>
--- a/src/test/test-data/AppBridgeTestData.xlsx
+++ b/src/test/test-data/AppBridgeTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="APPBRIDGE" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="78">
   <si>
     <t>API</t>
   </si>
@@ -78,15 +78,6 @@
     <t>status=200||errorCode=ab-error-101||errorMsg=SteamID can NOT be found</t>
   </si>
   <si>
-    <t>OPQA-XXXX1</t>
-  </si>
-  <si>
-    <t>OPQA-XXXX2</t>
-  </si>
-  <si>
-    <t>OPQA-XXXX3</t>
-  </si>
-  <si>
     <t>status=403</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t>Verify that user able to send article to endnote using  1PAPPBRIDGE API</t>
   </si>
   <si>
-    <t>OPQA-XXXX4</t>
-  </si>
-  <si>
     <t>/bridge/en/savedoctoen/wos/(OPQA-896_hits.hits._id)</t>
   </si>
   <si>
@@ -147,9 +135,6 @@
     <t>?query=Post&amp;size=1</t>
   </si>
   <si>
-    <t>OPQA-XXXX5</t>
-  </si>
-  <si>
     <t>status=200||type=posts||id=(OPQA-897_hits.hits._id)</t>
   </si>
   <si>
@@ -168,9 +153,6 @@
     <t>?query=biotechnology&amp;size=1</t>
   </si>
   <si>
-    <t>OPQA-XXXX6</t>
-  </si>
-  <si>
     <t>Verify that user able to send patents to endnote using  1PAPPBRIDGE API</t>
   </si>
   <si>
@@ -183,15 +165,9 @@
     <t>status=200||type=patents||id=(OPQA-898_hits.hits._id)</t>
   </si>
   <si>
-    <t>OPQA-XXXX7</t>
-  </si>
-  <si>
     <t>Verify that to get error status when passing wrong truid to 1PAPPBRIDGE send document API</t>
   </si>
   <si>
-    <t>OPQA-XXXX8</t>
-  </si>
-  <si>
     <t>Verify that to get error status when not passing truid to 1PAPPBRIDGE send document API</t>
   </si>
   <si>
@@ -216,9 +192,6 @@
     <t>Verify that to get error status when passing wrong document id to 1PAPPBRIDGE send document API</t>
   </si>
   <si>
-    <t>OPQA-XXXX9</t>
-  </si>
-  <si>
     <t>/bridge/en/savedoctoen/wos/(OPQA-896_hits.hits._id)1</t>
   </si>
   <si>
@@ -234,10 +207,49 @@
     <t>status=200||errorCode=ab-error-204||errorMsg=doc type is not suppored</t>
   </si>
   <si>
-    <t>OPQA-XXXX10</t>
-  </si>
-  <si>
     <t>status=200||truid=(SYS_USER1)||enRedirectUrl=https://app.qc.endnote.com/auth?token</t>
+  </si>
+  <si>
+    <t>OPQA-3493</t>
+  </si>
+  <si>
+    <t>OPQA-3494</t>
+  </si>
+  <si>
+    <t>OPQA-3495</t>
+  </si>
+  <si>
+    <t>OPQA-3496</t>
+  </si>
+  <si>
+    <t>OPQA-3497</t>
+  </si>
+  <si>
+    <t>OPQA-3498</t>
+  </si>
+  <si>
+    <t>OPQA-3499</t>
+  </si>
+  <si>
+    <t>OPQA-3500</t>
+  </si>
+  <si>
+    <t>OPQA-3501</t>
+  </si>
+  <si>
+    <t>OPQA-3502</t>
+  </si>
+  <si>
+    <t>OPQA-3503</t>
+  </si>
+  <si>
+    <t>OPQA-3504</t>
+  </si>
+  <si>
+    <t>OPQA-3505</t>
+  </si>
+  <si>
+    <t>OPQA-3506</t>
   </si>
 </sst>
 </file>
@@ -638,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L14"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -698,7 +710,7 @@
     </row>
     <row r="2" spans="1:12" ht="60">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -719,13 +731,13 @@
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" s="5" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="60">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>17</v>
@@ -749,10 +761,10 @@
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>13</v>
@@ -766,199 +778,199 @@
       <c r="F4" s="1"/>
       <c r="H4"/>
       <c r="J4" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45">
       <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
       <c r="J5" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H6"/>
       <c r="I6" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="1"/>
       <c r="J7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="45">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H8"/>
       <c r="I8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="1"/>
       <c r="J9" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H10"/>
       <c r="I10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="60">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H11"/>
       <c r="I11" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>19</v>
@@ -966,81 +978,81 @@
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F12" s="1"/>
       <c r="H12"/>
       <c r="I12" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="45">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H13"/>
       <c r="I13" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="45">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H14"/>
       <c r="I14" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1053,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1113,10 +1125,10 @@
     </row>
     <row r="2" spans="1:12" ht="60">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>
@@ -1131,63 +1143,63 @@
         <v>15</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="60">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1199,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1259,10 +1271,10 @@
     </row>
     <row r="2" spans="1:12" ht="60">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>
@@ -1277,63 +1289,63 @@
         <v>15</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="60">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified validations in 1PAPPBRIDGE
</commit_message>
<xml_diff>
--- a/src/test/test-data/AppBridgeTestData.xlsx
+++ b/src/test/test-data/AppBridgeTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="APPBRIDGE" sheetId="1" r:id="rId1"/>
@@ -171,15 +171,9 @@
     <t>Verify that to get error status when not passing truid to 1PAPPBRIDGE send document API</t>
   </si>
   <si>
-    <t>status=200||type=wos||id=(OPQA-897_hits.hits._id)||errorCode=ab-error-102||errorMsg=error out when retrieving endnote token</t>
-  </si>
-  <si>
     <t>status=200||truid=(SYS_USER1)||errorCode=ab-error-103||errorMsg=Endnote is under maintenance</t>
   </si>
   <si>
-    <t>status=200||type=wos||id=(OPQA-897_hits.hits._id)||errorCode=ab-error-103||errorMsg=Endnote is under maintenance</t>
-  </si>
-  <si>
     <t>Verify that to get error status when endnote is maintenance to 1PAPPBRIDGE EN redirect  API</t>
   </si>
   <si>
@@ -250,6 +244,12 @@
   </si>
   <si>
     <t>OPQA-3506</t>
+  </si>
+  <si>
+    <t>status=200||type=posts||id=(OPQA-897_hits.hits._id)||errorCode=ab-error-102||errorMsg=error out when retrieving endnote token</t>
+  </si>
+  <si>
+    <t>status=200||type=posts||id=(OPQA-897_hits.hits._id)||errorCode=ab-error-103||errorMsg=Endnote is under maintenance</t>
   </si>
 </sst>
 </file>
@@ -710,7 +710,7 @@
     </row>
     <row r="2" spans="1:12" ht="60">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -731,13 +731,13 @@
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="60">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>17</v>
@@ -761,7 +761,7 @@
     </row>
     <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
@@ -812,7 +812,7 @@
     </row>
     <row r="6" spans="1:12" ht="30">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>31</v>
@@ -868,7 +868,7 @@
     </row>
     <row r="8" spans="1:12" ht="45">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>40</v>
@@ -924,7 +924,7 @@
     </row>
     <row r="10" spans="1:12" ht="45">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>45</v>
@@ -951,7 +951,7 @@
     </row>
     <row r="11" spans="1:12" ht="60">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>49</v>
@@ -978,7 +978,7 @@
     </row>
     <row r="12" spans="1:12" ht="30">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>50</v>
@@ -1003,16 +1003,16 @@
     </row>
     <row r="13" spans="1:12" ht="45">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>33</v>
@@ -1025,21 +1025,21 @@
         <v>24</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="45">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>33</v>
@@ -1052,7 +1052,7 @@
         <v>24</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1065,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="2" spans="1:12" ht="60">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>22</v>
@@ -1142,6 +1142,7 @@
       <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="H2"/>
       <c r="J2" s="5" t="s">
         <v>23</v>
       </c>
@@ -1177,10 +1178,10 @@
     </row>
     <row r="4" spans="1:12" ht="60">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>13</v>
@@ -1199,7 +1200,7 @@
         <v>35</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1211,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1271,10 +1272,10 @@
     </row>
     <row r="2" spans="1:12" ht="60">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>
@@ -1289,7 +1290,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75">
@@ -1323,10 +1324,10 @@
     </row>
     <row r="4" spans="1:12" ht="60">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>13</v>
@@ -1345,7 +1346,7 @@
         <v>35</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed tests related to posts,patents and people
</commit_message>
<xml_diff>
--- a/src/test/test-data/AppBridgeTestData.xlsx
+++ b/src/test/test-data/AppBridgeTestData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\API Project\LatestAPIs\1p-api-automation\src\test\test-data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="APPBRIDGE" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="68">
   <si>
     <t>API</t>
   </si>
@@ -123,24 +128,6 @@
     <t>?query=Post&amp;size=1</t>
   </si>
   <si>
-    <t>Verify that user able to send post to endnote using  1PAPPBRIDGE API</t>
-  </si>
-  <si>
-    <t>OPQA-898</t>
-  </si>
-  <si>
-    <t>Verify that to get patents for query</t>
-  </si>
-  <si>
-    <t>/patents/search</t>
-  </si>
-  <si>
-    <t>?query=biotechnology&amp;size=1</t>
-  </si>
-  <si>
-    <t>Verify that user able to send patents to endnote using  1PAPPBRIDGE API</t>
-  </si>
-  <si>
     <t>Verify that to get error status when passing wrong truid to 1PAPPBRIDGE send document API</t>
   </si>
   <si>
@@ -186,12 +173,6 @@
     <t>OPQA-3496</t>
   </si>
   <si>
-    <t>OPQA-3497</t>
-  </si>
-  <si>
-    <t>OPQA-3498</t>
-  </si>
-  <si>
     <t>OPQA-3499</t>
   </si>
   <si>
@@ -225,18 +206,9 @@
     <t>status=200||type=wos||id=(OPQA-896_hits.id)</t>
   </si>
   <si>
-    <t>status=200||type=posts||id=(OPQA-897_hits.id)</t>
-  </si>
-  <si>
     <t>/bridge/en/savedoctoen/posts/(OPQA-897_hits.id)</t>
   </si>
   <si>
-    <t>status=200||type=patents||id=(OPQA-898_hits.id)</t>
-  </si>
-  <si>
-    <t>/bridge/en/savedoctoen/patents/(OPQA-898_hits.id)</t>
-  </si>
-  <si>
     <t>/bridge/en/savedoctoen/wos/(OPQA-896_hits.id)1</t>
   </si>
   <si>
@@ -250,13 +222,17 @@
   </si>
   <si>
     <t>status=200||type=posts||id=(OPQA-897_hits.id)||errorCode=ab-error-103||errorMsg=Endnote is under maintenance</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,6 +336,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -406,7 +390,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -438,9 +422,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -472,6 +457,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -647,30 +633,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="57.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="59.28515625" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="25.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="44.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="57.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="59.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="25.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -708,9 +694,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
@@ -731,13 +717,16 @@
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="60">
+      <c r="L2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>17</v>
@@ -754,14 +743,20 @@
       <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="G3"/>
       <c r="H3"/>
+      <c r="I3"/>
       <c r="J3" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="30">
+      <c r="K3"/>
+      <c r="L3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>21</v>
@@ -776,12 +771,18 @@
         <v>16</v>
       </c>
       <c r="F4" s="1"/>
+      <c r="G4"/>
       <c r="H4"/>
+      <c r="I4"/>
       <c r="J4" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="45">
+      <c r="K4"/>
+      <c r="L4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
@@ -789,7 +790,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>26</v>
@@ -807,12 +808,15 @@
         <v>28</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="30">
+        <v>58</v>
+      </c>
+      <c r="L5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>29</v>
@@ -821,7 +825,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>30</v>
@@ -829,111 +833,125 @@
       <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="G6"/>
       <c r="H6"/>
       <c r="I6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75">
+        <v>60</v>
+      </c>
+      <c r="K6"/>
+      <c r="L6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="1"/>
-      <c r="J7" t="s">
-        <v>28</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="30">
+        <v>50</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7"/>
+      <c r="L7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8"/>
+      <c r="L8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H8"/>
-      <c r="I8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="30">
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9"/>
+      <c r="L9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>30</v>
@@ -941,118 +959,17 @@
       <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="G10"/>
       <c r="H10"/>
-      <c r="I10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="60">
-      <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="I10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10"/>
+      <c r="L10" t="s">
         <v>67</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11"/>
-      <c r="I11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="30">
-      <c r="A12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="H12"/>
-      <c r="I12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="45">
-      <c r="A13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13"/>
-      <c r="I13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="45">
-      <c r="A14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14"/>
-      <c r="I14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1062,30 +979,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="57.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="59.28515625" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="33.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="44.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="57.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="59.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="33.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1123,9 +1040,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>22</v>
@@ -1147,7 +1064,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1155,7 +1072,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>33</v>
@@ -1173,21 +1090,21 @@
         <v>28</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>30</v>
@@ -1200,7 +1117,7 @@
         <v>31</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1209,30 +1126,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="44.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="57.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="59.28515625" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="36.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="44.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="57.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="30.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="59.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="36.5703125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1270,12 +1187,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="60">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>
@@ -1290,10 +1207,10 @@
         <v>15</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1301,7 +1218,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>33</v>
@@ -1319,21 +1236,21 @@
         <v>28</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="60">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>30</v>
@@ -1346,7 +1263,7 @@
         <v>31</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>